<commit_message>
Updated the code with changes
</commit_message>
<xml_diff>
--- a/coempt_automation/src/test/resources/dataSheets/ResulProcess.xlsx
+++ b/coempt_automation/src/test/resources/dataSheets/ResulProcess.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Exam Series</t>
   </si>
@@ -71,9 +71,6 @@
     <t>PART-II</t>
   </si>
   <si>
-    <t>54</t>
-  </si>
-  <si>
     <t>62</t>
   </si>
   <si>
@@ -113,16 +110,28 @@
     <t>34</t>
   </si>
   <si>
-    <t>49.98</t>
-  </si>
-  <si>
-    <t>149.94</t>
-  </si>
-  <si>
-    <t>149.99</t>
-  </si>
-  <si>
-    <t>null</t>
+    <t>55</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>335</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -451,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +506,7 @@
         <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>13</v>
@@ -505,7 +514,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -523,22 +532,22 @@
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="K2" s="1">
         <v>200</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -558,25 +567,25 @@
         <v>2018</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -637,22 +646,22 @@
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="1">
-        <v>335</v>
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -678,10 +687,10 @@
         <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J6" s="1">
         <v>187</v>

</xml_diff>

<commit_message>
pdf validation along with report
</commit_message>
<xml_diff>
--- a/coempt_automation/src/test/resources/dataSheets/ResulProcess.xlsx
+++ b/coempt_automation/src/test/resources/dataSheets/ResulProcess.xlsx
@@ -131,7 +131,7 @@
     <t>335</t>
   </si>
   <si>
-    <t>12</t>
+    <t>54</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>